<commit_message>
Première mise en place d'SQL
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_03_28.xlsx
+++ b/Excel/TI/Mon_TI_2024_03_28.xlsx
@@ -628,12 +628,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dejounte Murray</t>
+          <t>Jaylen Brown</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -642,25 +642,21 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>38.6</v>
+        <v>39.8</v>
       </c>
       <c r="G2" t="n">
-        <v>37.9</v>
+        <v>37.5</v>
       </c>
       <c r="H2" t="n">
         <v>32.1</v>
       </c>
       <c r="I2" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>2</v>
@@ -669,45 +665,43 @@
         <v>3</v>
       </c>
       <c r="M2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N2" t="n">
-        <v>59</v>
-      </c>
-      <c r="O2" t="n">
-        <v>42</v>
+        <v>25</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P2" t="n">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="Q2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R2" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="U2" t="n">
-        <v>-7.8</v>
-      </c>
-      <c r="V2" t="n">
-        <v>11</v>
-      </c>
+        <v>-2.2</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -716,36 +710,32 @@
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>-3</v>
+        <v>25</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB2" t="n">
+        <v>28</v>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AD2" t="n">
+        <v>26</v>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -755,7 +745,7 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
@@ -765,29 +755,29 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>SAC</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jaylen Brown</t>
+          <t>Dejounte Murray</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -796,24 +786,28 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F3" t="n">
-        <v>40.8</v>
+        <v>38.8</v>
       </c>
       <c r="G3" t="n">
-        <v>37.3</v>
+        <v>37.1</v>
       </c>
       <c r="H3" t="n">
         <v>32.2</v>
       </c>
       <c r="I3" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" t="n">
         <v>3</v>
@@ -821,43 +815,43 @@
       <c r="M3" t="n">
         <v>7</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="N3" t="n">
+        <v>49</v>
       </c>
       <c r="O3" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="P3" t="n">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="Q3" t="n">
-        <v>45</v>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>42</v>
+      </c>
+      <c r="R3" t="n">
+        <v>16</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>-2.1</v>
-      </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-8</v>
+      </c>
+      <c r="V3" t="n">
+        <v>11</v>
+      </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -870,11 +864,11 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB3" t="n">
-        <v>26</v>
+        <v>-3</v>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
@@ -888,12 +882,12 @@
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
@@ -903,7 +897,7 @@
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
@@ -913,17 +907,17 @@
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>DAL</t>
         </is>
       </c>
     </row>
@@ -946,13 +940,13 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>29.8</v>
+        <v>26</v>
       </c>
       <c r="G4" t="n">
-        <v>35.3</v>
+        <v>35.1</v>
       </c>
       <c r="H4" t="n">
-        <v>33</v>
+        <v>32.8</v>
       </c>
       <c r="I4" t="n">
         <v>7</v>
@@ -961,40 +955,38 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
         <v>3</v>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>24</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
         <v>28</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>15</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>33</v>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>@</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
@@ -1010,21 +1002,19 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="Z4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
         <v>44</v>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
@@ -1088,7 +1078,11 @@
           <t>Khris Middleton</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Probable</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>F</t>
@@ -1096,19 +1090,19 @@
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>26</v>
+        <v>25.8</v>
       </c>
       <c r="G5" t="n">
-        <v>26.8</v>
+        <v>25.4</v>
       </c>
       <c r="H5" t="n">
-        <v>23.9</v>
+        <v>23.8</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
@@ -1120,31 +1114,29 @@
         <v>1</v>
       </c>
       <c r="N5" t="n">
+        <v>17</v>
+      </c>
+      <c r="O5" t="n">
         <v>23</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P5" t="n">
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
         <v>41</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>36</v>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>@</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>-0.7</v>
+        <v>-0.6</v>
       </c>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>

</xml_diff>